<commit_message>
Several file changes were to correct the mu in vitamin d. Also lots of changes develop the new graphing tools in aggRun.R
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/comp_fct_beans_cbean.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/comp_fct_beans_cbean.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-30860" yWindow="-320" windowWidth="28200" windowHeight="10400"/>
+    <workbookView xWindow="-29020" yWindow="-2000" windowWidth="28200" windowHeight="10400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -209,7 +209,7 @@
     <t>Composite</t>
   </si>
   <si>
-    <t>vit_d_μg</t>
+    <t>vit_d_µg</t>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
   <dimension ref="A1:AR16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AN1" sqref="AN1"/>
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>